<commit_message>
Masked machine ID version check to look at bottom 4 bits only.
</commit_message>
<xml_diff>
--- a/docs/baud prescalar.xlsx
+++ b/docs/baud prescalar.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\Visual Studio 2015\Projects\nget\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEE1153-5629-4D69-ACAF-7FFD57E6F465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA6F12-E05E-4373-BE42-99372BC9949F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1065" windowWidth="20490" windowHeight="9555" activeTab="2" xr2:uid="{39877972-80F9-4A2A-BBD8-642929DB01CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{39877972-80F9-4A2A-BBD8-642929DB01CE}"/>
   </bookViews>
   <sheets>
     <sheet name="115200" sheetId="2" r:id="rId1"/>
-    <sheet name="1152000" sheetId="4" r:id="rId2"/>
-    <sheet name="1152000 Tim" sheetId="5" r:id="rId3"/>
-    <sheet name="115273" sheetId="3" r:id="rId4"/>
-    <sheet name="Test" sheetId="1" r:id="rId5"/>
+    <sheet name="77800 " sheetId="6" r:id="rId2"/>
+    <sheet name="1152000" sheetId="4" r:id="rId3"/>
+    <sheet name="1152000 Tim" sheetId="5" r:id="rId4"/>
+    <sheet name="115273" sheetId="3" r:id="rId5"/>
+    <sheet name="Test" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="20">
   <si>
     <t>DEFW 243,248,256,260,269,278,286,234</t>
   </si>
@@ -1009,6 +1010,486 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34DB301-0F6F-43DA-8EBE-3E7C343DF61F}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="9.140625" style="6"/>
+    <col min="10" max="12" width="9.140625" style="8"/>
+    <col min="13" max="13" width="53.140625" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11">
+        <v>77800</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>28000000</v>
+      </c>
+      <c r="D2">
+        <f>INT(C2/D$1)</f>
+        <v>359</v>
+      </c>
+      <c r="E2" s="6" t="str">
+        <f>DEC2HEX(D2, 4)</f>
+        <v>0167</v>
+      </c>
+      <c r="F2" s="6" t="str">
+        <f>HEX2BIN(RIGHT(E2, 2), 8)</f>
+        <v>01100111</v>
+      </c>
+      <c r="G2" s="6" t="str">
+        <f>HEX2BIN(LEFT(E2, 2), 8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="H2" s="6" t="str">
+        <f>RIGHT(F2, 7)</f>
+        <v>1100111</v>
+      </c>
+      <c r="I2" s="6" t="str">
+        <f>RIGHT(G2, 6) &amp; LEFT(F2, 1)</f>
+        <v>0000010</v>
+      </c>
+      <c r="J2" s="8" t="str">
+        <f>"0" &amp; H2</f>
+        <v>01100111</v>
+      </c>
+      <c r="K2" s="8" t="str">
+        <f>"1" &amp; I2</f>
+        <v>10000010</v>
+      </c>
+      <c r="L2" s="8" t="str">
+        <f>BIN2HEX(K2, 2) &amp; BIN2HEX(J2, 2)</f>
+        <v>8267</v>
+      </c>
+      <c r="M2" s="10" t="str">
+        <f>"dw $" &amp; L2</f>
+        <v>dw $8267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <f t="shared" ref="A3:A9" si="0">A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>28571429</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="1">INT(C3/D$1)</f>
+        <v>367</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f t="shared" ref="E3:E9" si="2">DEC2HEX(D3, 4)</f>
+        <v>016F</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f t="shared" ref="F3:F9" si="3">HEX2BIN(RIGHT(E3, 2), 8)</f>
+        <v>01101111</v>
+      </c>
+      <c r="G3" s="6" t="str">
+        <f t="shared" ref="G3:G9" si="4">HEX2BIN(LEFT(E3, 2), 8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="H3" s="6" t="str">
+        <f t="shared" ref="H3:H9" si="5">RIGHT(F3, 7)</f>
+        <v>1101111</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f t="shared" ref="I3:I9" si="6">RIGHT(G3, 6) &amp; LEFT(F3, 1)</f>
+        <v>0000010</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f t="shared" ref="J3:J9" si="7">"0" &amp; H3</f>
+        <v>01101111</v>
+      </c>
+      <c r="K3" s="8" t="str">
+        <f t="shared" ref="K3:K9" si="8">"1" &amp; I3</f>
+        <v>10000010</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f t="shared" ref="L3:L9" si="9">BIN2HEX(K3, 2) &amp; BIN2HEX(J3, 2)</f>
+        <v>826F</v>
+      </c>
+      <c r="M3" s="10" t="str">
+        <f>M2 &amp; ", $" &amp; L3</f>
+        <v>dw $8267, $826F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>29464286</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>378</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>017A</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01111010</v>
+      </c>
+      <c r="G4" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H4" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1111010</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000010</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>01111010</v>
+      </c>
+      <c r="K4" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000010</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>827A</v>
+      </c>
+      <c r="M4" s="10" t="str">
+        <f t="shared" ref="M4:M9" si="10">M3 &amp; ", $" &amp; L4</f>
+        <v>dw $8267, $826F, $827A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30000000</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>385</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>0181</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>10000001</v>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H5" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>0000001</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000011</v>
+      </c>
+      <c r="J5" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>00000001</v>
+      </c>
+      <c r="K5" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000011</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>8301</v>
+      </c>
+      <c r="M5" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>dw $8267, $826F, $827A, $8301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>31000000</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>398</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>018E</v>
+      </c>
+      <c r="F6" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>10001110</v>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H6" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>0001110</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000011</v>
+      </c>
+      <c r="J6" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>00001110</v>
+      </c>
+      <c r="K6" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000011</v>
+      </c>
+      <c r="L6" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>830E</v>
+      </c>
+      <c r="M6" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>dw $8267, $826F, $827A, $8301, $830E</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>32000000</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>411</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>019B</v>
+      </c>
+      <c r="F7" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>10011011</v>
+      </c>
+      <c r="G7" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H7" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>0011011</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000011</v>
+      </c>
+      <c r="J7" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>00011011</v>
+      </c>
+      <c r="K7" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000011</v>
+      </c>
+      <c r="L7" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>831B</v>
+      </c>
+      <c r="M7" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>dw $8267, $826F, $827A, $8301, $830E, $831B</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>33000000</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>424</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>01A8</v>
+      </c>
+      <c r="F8" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>10101000</v>
+      </c>
+      <c r="G8" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H8" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>0101000</v>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000011</v>
+      </c>
+      <c r="J8" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>00101000</v>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000011</v>
+      </c>
+      <c r="L8" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>8328</v>
+      </c>
+      <c r="M8" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>dw $8267, $826F, $827A, $8301, $830E, $831B, $8328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>27000000</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>347</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>015B</v>
+      </c>
+      <c r="F9" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01011011</v>
+      </c>
+      <c r="G9" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>00000001</v>
+      </c>
+      <c r="H9" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>1011011</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>0000010</v>
+      </c>
+      <c r="J9" s="8" t="str">
+        <f t="shared" si="7"/>
+        <v>01011011</v>
+      </c>
+      <c r="K9" s="8" t="str">
+        <f t="shared" si="8"/>
+        <v>10000010</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f t="shared" si="9"/>
+        <v>825B</v>
+      </c>
+      <c r="M9" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v>dw $8267, $826F, $827A, $8301, $830E, $831B, $8328, $825B</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE7F23D-5CD4-49E9-93A7-232448E27695}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -1488,11 +1969,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AFC565-AFC5-4178-A6C0-CAB736A4F44C}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
@@ -1916,7 +2397,7 @@
         <v>27000000</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D3:D9" si="10">INT(C9/D$1)</f>
+        <f t="shared" ref="D9" si="10">INT(C9/D$1)</f>
         <v>23</v>
       </c>
       <c r="E9" s="6" t="str">
@@ -1962,7 +2443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{757B6398-5630-44FA-9E83-BDAF0E237CE5}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2442,7 +2923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5182CB9A-203F-43B9-A2A3-3FE182BA0142}">
   <dimension ref="A1:Q13"/>
   <sheetViews>

</xml_diff>